<commit_message>
Simple field types validation, and fixing the constraint entity builder.
</commit_message>
<xml_diff>
--- a/resources/files/Constraints/MasterData.xlsx
+++ b/resources/files/Constraints/MasterData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8970" windowHeight="4635" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8970" windowHeight="4635" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="hrd_company" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="62">
   <si>
     <t>Name Field</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Company Code</t>
   </si>
   <si>
-    <t>1 = True, 0 = False</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>Minimum Living Cost</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,15 +651,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -673,7 +671,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -687,7 +685,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -737,7 +735,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -751,7 +749,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -763,7 +761,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -775,7 +773,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -787,7 +785,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -799,7 +797,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -811,7 +809,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -858,7 +856,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -872,7 +870,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -886,7 +884,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -935,7 +933,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -949,7 +947,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -963,7 +961,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1012,7 +1010,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1026,7 +1024,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1040,35 +1038,35 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1077,12 +1075,12 @@
         <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1094,7 +1092,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -1106,7 +1104,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -1118,7 +1116,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -1130,7 +1128,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
@@ -1149,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1175,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1191,7 +1189,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1212,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1240,7 +1238,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1254,7 +1252,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1268,7 +1266,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1315,7 +1313,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1329,7 +1327,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1378,7 +1376,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1392,7 +1390,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1406,7 +1404,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1455,7 +1453,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1469,7 +1467,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1483,7 +1481,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1497,7 +1495,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1546,7 +1544,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1560,7 +1558,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1574,7 +1572,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1588,7 +1586,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1602,7 +1600,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1651,7 +1649,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1665,7 +1663,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1679,7 +1677,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1693,7 +1691,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1707,7 +1705,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1721,7 +1719,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1770,7 +1768,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1784,7 +1782,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1796,7 +1794,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1808,7 +1806,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1820,7 +1818,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1867,7 +1865,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1881,7 +1879,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1895,7 +1893,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -1907,7 +1905,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -1919,7 +1917,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -1931,7 +1929,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -1978,7 +1976,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1992,7 +1990,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -2006,7 +2004,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2018,7 +2016,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
@@ -2030,7 +2028,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2042,7 +2040,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>

</xml_diff>